<commit_message>
Made some to excel file regarding the attribute names
</commit_message>
<xml_diff>
--- a/MVC excel Assig.xlsx
+++ b/MVC excel Assig.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531441\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531524\Desktop\MVC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820512BA-1B4A-4F69-AD66-4E6CD6D88C67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="80">
   <si>
     <t>DegreeId</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>DegreeRequirementId</t>
-  </si>
-  <si>
-    <t>RequirementId</t>
   </si>
   <si>
     <t>DegreePlanTermRequirementId</t>
@@ -285,7 +282,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -605,17 +602,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -680,7 +678,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -853,11 +851,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1412,11 +1410,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,16 +1426,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2678,7 +2676,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2694,19 +2692,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2720,10 +2718,10 @@
         <v>531441</v>
       </c>
       <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
         <v>48</v>
-      </c>
-      <c r="E2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2737,10 +2735,10 @@
         <v>531441</v>
       </c>
       <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
         <v>50</v>
-      </c>
-      <c r="E3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2754,10 +2752,10 @@
         <v>531524</v>
       </c>
       <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
         <v>48</v>
-      </c>
-      <c r="E4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2771,10 +2769,10 @@
         <v>531524</v>
       </c>
       <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
         <v>50</v>
-      </c>
-      <c r="E5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2788,10 +2786,10 @@
         <v>531506</v>
       </c>
       <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
         <v>48</v>
-      </c>
-      <c r="E6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2805,10 +2803,10 @@
         <v>531506</v>
       </c>
       <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
         <v>50</v>
-      </c>
-      <c r="E7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2822,10 +2820,10 @@
         <v>530469</v>
       </c>
       <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
         <v>48</v>
-      </c>
-      <c r="E8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2839,10 +2837,10 @@
         <v>530469</v>
       </c>
       <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
         <v>50</v>
-      </c>
-      <c r="E9" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2851,7 +2849,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2865,16 +2863,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" t="s">
-        <v>54</v>
       </c>
       <c r="E1">
         <v>919</v>
@@ -2885,10 +2883,10 @@
         <v>531441</v>
       </c>
       <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
         <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
       </c>
       <c r="D2">
         <v>531441</v>
@@ -2902,10 +2900,10 @@
         <v>531524</v>
       </c>
       <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
         <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
       </c>
       <c r="D3">
         <v>531524</v>
@@ -2919,10 +2917,10 @@
         <v>530469</v>
       </c>
       <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
         <v>59</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
       </c>
       <c r="D4">
         <v>530469</v>
@@ -2936,10 +2934,10 @@
         <v>531506</v>
       </c>
       <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
         <v>61</v>
-      </c>
-      <c r="C5" t="s">
-        <v>62</v>
       </c>
       <c r="D5">
         <v>531506</v>
@@ -2954,7 +2952,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
@@ -2968,16 +2966,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
         <v>63</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>64</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>65</v>
-      </c>
-      <c r="D1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2991,7 +2989,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3005,7 +3003,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3019,7 +3017,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3033,7 +3031,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3047,7 +3045,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3061,7 +3059,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3075,7 +3073,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3089,7 +3087,7 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3103,7 +3101,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3117,7 +3115,7 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3131,7 +3129,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3145,7 +3143,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3159,7 +3157,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3173,7 +3171,7 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3187,7 +3185,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3201,7 +3199,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3215,7 +3213,7 @@
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3229,7 +3227,7 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3243,7 +3241,7 @@
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3257,7 +3255,7 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3271,7 +3269,7 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3285,7 +3283,7 @@
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3299,7 +3297,7 @@
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3313,7 +3311,7 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3327,7 +3325,7 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3341,7 +3339,7 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3355,7 +3353,7 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3369,7 +3367,7 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3383,7 +3381,7 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3397,7 +3395,7 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3411,7 +3409,7 @@
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3425,7 +3423,7 @@
         <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3439,7 +3437,7 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3453,7 +3451,7 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3467,7 +3465,7 @@
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3481,7 +3479,7 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3495,7 +3493,7 @@
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3509,7 +3507,7 @@
         <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -3518,10 +3516,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Made changes in excel
</commit_message>
<xml_diff>
--- a/MVC excel Assig.xlsx
+++ b/MVC excel Assig.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,8 @@
     <sheet name="DegreePlan" sheetId="5" r:id="rId5"/>
     <sheet name="Student" sheetId="6" r:id="rId6"/>
     <sheet name="StudentTerm" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="79">
   <si>
     <t>DegreeId</t>
   </si>
@@ -252,9 +251,6 @@
     <t>Fall 2018</t>
   </si>
   <si>
-    <t>Spring2019</t>
-  </si>
-  <si>
     <t>Summer 2019</t>
   </si>
   <si>
@@ -262,9 +258,6 @@
   </si>
   <si>
     <t>Fall 2019</t>
-  </si>
-  <si>
-    <t>Spring2020</t>
   </si>
   <si>
     <t>Summer 2020</t>
@@ -1415,8 +1408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,7 +1511,7 @@
         <v>10</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1560,7 +1553,7 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -1588,7 +1581,7 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>692</v>
@@ -1896,7 +1889,7 @@
         <v>12</v>
       </c>
       <c r="C34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D34">
         <v>692</v>
@@ -2134,7 +2127,7 @@
         <v>14</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -2176,7 +2169,7 @@
         <v>14</v>
       </c>
       <c r="C54">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D54">
         <v>10</v>
@@ -2204,7 +2197,7 @@
         <v>14</v>
       </c>
       <c r="C56">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D56">
         <v>692</v>
@@ -2470,7 +2463,7 @@
         <v>16</v>
       </c>
       <c r="C75">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D75">
         <v>691</v>
@@ -2512,7 +2505,7 @@
         <v>16</v>
       </c>
       <c r="C78">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D78">
         <v>692</v>
@@ -2955,10 +2948,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3044,10 +3037,10 @@
         <v>531441</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3055,10 +3048,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>531441</v>
+        <v>531524</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
         <v>68</v>
@@ -3069,10 +3062,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>531441</v>
+        <v>531524</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
         <v>69</v>
@@ -3083,10 +3076,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>531441</v>
+        <v>531524</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
         <v>70</v>
@@ -3097,13 +3090,13 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>531441</v>
+        <v>531524</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3111,13 +3104,13 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>531441</v>
+        <v>531524</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3125,13 +3118,13 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>531524</v>
+        <v>530469</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3139,13 +3132,13 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>531524</v>
+        <v>530469</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3153,13 +3146,13 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>531524</v>
+        <v>530469</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3167,7 +3160,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>531524</v>
+        <v>530469</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -3181,13 +3174,13 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>531524</v>
+        <v>530469</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3195,13 +3188,13 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>531524</v>
+        <v>531506</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3209,13 +3202,13 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>531524</v>
+        <v>531506</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3223,13 +3216,13 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>531524</v>
+        <v>531506</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3237,13 +3230,13 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>531524</v>
+        <v>531506</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3251,280 +3244,16 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>530469</v>
+        <v>531506</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>530469</v>
-      </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>530469</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>530469</v>
-      </c>
-      <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>530469</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>530469</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>530469</v>
-      </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="D27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>530469</v>
-      </c>
-      <c r="C28">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>530469</v>
-      </c>
-      <c r="C29">
-        <v>5</v>
-      </c>
-      <c r="D29" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>530469</v>
-      </c>
-      <c r="C30">
-        <v>6</v>
-      </c>
-      <c r="D30" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>531506</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>531506</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-      <c r="D32" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>531506</v>
-      </c>
-      <c r="C33">
-        <v>3</v>
-      </c>
-      <c r="D33" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>531506</v>
-      </c>
-      <c r="C34">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>531506</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36">
-        <v>531506</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37">
-        <v>531506</v>
-      </c>
-      <c r="C37">
-        <v>3</v>
-      </c>
-      <c r="D37" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>531506</v>
-      </c>
-      <c r="C38">
-        <v>4</v>
-      </c>
-      <c r="D38" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39">
-        <v>531506</v>
-      </c>
-      <c r="C39">
-        <v>5</v>
-      </c>
-      <c r="D39" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Assignment Module 4: Working with EF Completed Some part of models and data initializes and also edited Excel and need to work on more for submission.
</commit_message>
<xml_diff>
--- a/MVC excel Assig.xlsx
+++ b/MVC excel Assig.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531441\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531441\Documents\C# and .Net\MVC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -36,16 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="79">
-  <si>
-    <t>DegreeId</t>
-  </si>
-  <si>
-    <t>DegreeAbrrev(unique,max 6 characters)</t>
-  </si>
-  <si>
-    <t>DegreeName(unique, max 20 characters)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
   <si>
     <t>ACS+2</t>
   </si>
@@ -152,24 +143,9 @@
     <t>GDP2</t>
   </si>
   <si>
-    <t>DegreeRequirementId</t>
-  </si>
-  <si>
-    <t>RequirementId</t>
-  </si>
-  <si>
-    <t>DegreePlanTermRequirementId</t>
-  </si>
-  <si>
     <t>DegreePlanID</t>
   </si>
   <si>
-    <t>TermId</t>
-  </si>
-  <si>
-    <t>DegreePlanId</t>
-  </si>
-  <si>
     <t>DegreeID</t>
   </si>
   <si>
@@ -227,18 +203,12 @@
     <t>Thallada</t>
   </si>
   <si>
-    <t>StudentTermId</t>
-  </si>
-  <si>
     <t>StudentID</t>
   </si>
   <si>
     <t>Term</t>
   </si>
   <si>
-    <t>Term Label</t>
-  </si>
-  <si>
     <t>Fall 2017</t>
   </si>
   <si>
@@ -273,6 +243,45 @@
   </si>
   <si>
     <t>Summer 2021</t>
+  </si>
+  <si>
+    <t>opening</t>
+  </si>
+  <si>
+    <t>ending</t>
+  </si>
+  <si>
+    <t>new Degree{</t>
+  </si>
+  <si>
+    <t>},</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>DegreeAbrrev</t>
+  </si>
+  <si>
+    <t>DegreeName</t>
+  </si>
+  <si>
+    <t>DegreeRequirementID</t>
+  </si>
+  <si>
+    <t>DegreePlanTermRequirementID</t>
+  </si>
+  <si>
+    <t>TermID</t>
+  </si>
+  <si>
+    <t>919(SID)</t>
+  </si>
+  <si>
+    <t>StudentTermID</t>
+  </si>
+  <si>
+    <t>TermLabel</t>
   </si>
 </sst>
 </file>
@@ -599,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,59 +620,90 @@
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="str">
+        <f>D2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"='"&amp;B2&amp;"','"&amp;$C$1&amp;"='"&amp;C2&amp;"'),"</f>
+        <v>new Degree{DegreeID=1,DegreeAbrrev='ACS+2','DegreeName='MS ACS +2 '),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F5" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"='"&amp;B3&amp;"','"&amp;$C$1&amp;"='"&amp;C3&amp;"'),"</f>
+        <v>DegreeID=2,DegreeAbrrev='ACS+DB','DegreeName='MS ACS +DB'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>DegreeID=3,DegreeAbrrev='ACS+NF','DegreeName='MS ACS+NF'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>DegreeID=4,DegreeAbrrev='ACS','DegreeName='MS ACS'),</v>
       </c>
     </row>
   </sheetData>
@@ -676,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,13 +728,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -702,10 +742,10 @@
         <v>460</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -713,10 +753,10 @@
         <v>356</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -724,10 +764,10 @@
         <v>542</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -735,10 +775,10 @@
         <v>563</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -746,10 +786,10 @@
         <v>560</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -757,10 +797,10 @@
         <v>555</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -768,10 +808,10 @@
         <v>618</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -779,10 +819,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -790,10 +830,10 @@
         <v>664</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -801,10 +841,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -812,10 +852,10 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -823,10 +863,10 @@
         <v>691</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -834,10 +874,10 @@
         <v>692</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -849,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,13 +902,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1408,8 +1448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,16 +1461,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2675,7 +2715,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2687,19 +2727,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2713,10 +2753,10 @@
         <v>531441</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2730,10 +2770,10 @@
         <v>531441</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2747,10 +2787,10 @@
         <v>531524</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2764,10 +2804,10 @@
         <v>531524</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2781,10 +2821,10 @@
         <v>531506</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2798,10 +2838,10 @@
         <v>531506</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2815,10 +2855,10 @@
         <v>530469</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2832,10 +2872,10 @@
         <v>530469</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2848,7 +2888,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2858,19 +2898,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" t="s">
-        <v>53</v>
-      </c>
       <c r="D1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1">
-        <v>919</v>
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2878,10 +2918,10 @@
         <v>531441</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D2">
         <v>531441</v>
@@ -2895,10 +2935,10 @@
         <v>531524</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D3">
         <v>531524</v>
@@ -2912,10 +2952,10 @@
         <v>530469</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D4">
         <v>530469</v>
@@ -2929,10 +2969,10 @@
         <v>531506</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D5">
         <v>531506</v>
@@ -2951,7 +2991,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2961,16 +3001,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2984,7 +3024,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2998,7 +3038,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3012,7 +3052,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3026,7 +3066,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3040,7 +3080,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3054,7 +3094,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3068,7 +3108,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3082,7 +3122,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3096,7 +3136,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3110,7 +3150,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3124,7 +3164,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3138,7 +3178,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3152,7 +3192,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3166,7 +3206,7 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3180,7 +3220,7 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3194,7 +3234,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3208,7 +3248,7 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3222,7 +3262,7 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3236,7 +3276,7 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3250,7 +3290,7 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated excel sheet with formulas and generated code
</commit_message>
<xml_diff>
--- a/MVC excel Assig.xlsx
+++ b/MVC excel Assig.xlsx
@@ -5,38 +5,42 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531441\Documents\C# and .Net\MVC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S530469\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
     <sheet name="Requirement" sheetId="2" r:id="rId2"/>
     <sheet name="DegreeRequirement" sheetId="3" r:id="rId3"/>
-    <sheet name="DegreeplanTermRequirement" sheetId="4" r:id="rId4"/>
+    <sheet name="DegreePlanTermRequirement" sheetId="4" r:id="rId4"/>
     <sheet name="DegreePlan" sheetId="5" r:id="rId5"/>
     <sheet name="Student" sheetId="6" r:id="rId6"/>
     <sheet name="StudentTerm" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="93">
+  <si>
+    <t>DegreeId</t>
+  </si>
+  <si>
+    <t>DegreeAbrrev(unique,max 6 characters)</t>
+  </si>
+  <si>
+    <t>DegreeName(unique, max 20 characters)</t>
+  </si>
   <si>
     <t>ACS+2</t>
   </si>
@@ -143,21 +147,30 @@
     <t>GDP2</t>
   </si>
   <si>
+    <t>DegreeRequirementId</t>
+  </si>
+  <si>
+    <t>RequirementId</t>
+  </si>
+  <si>
+    <t>DegreePlanTermRequirementId</t>
+  </si>
+  <si>
     <t>DegreePlanID</t>
   </si>
   <si>
+    <t>TermId</t>
+  </si>
+  <si>
+    <t>DegreePlanId</t>
+  </si>
+  <si>
     <t>DegreeID</t>
   </si>
   <si>
     <t>StudentId</t>
   </si>
   <si>
-    <t>DegreePlanAbbrev(u,8)</t>
-  </si>
-  <si>
-    <t>DegreePlanName(u,20)</t>
-  </si>
-  <si>
     <t>No summer off</t>
   </si>
   <si>
@@ -203,12 +216,18 @@
     <t>Thallada</t>
   </si>
   <si>
+    <t>StudentTermId</t>
+  </si>
+  <si>
     <t>StudentID</t>
   </si>
   <si>
     <t>Term</t>
   </si>
   <si>
+    <t>Term Label</t>
+  </si>
+  <si>
     <t>Fall 2017</t>
   </si>
   <si>
@@ -245,43 +264,52 @@
     <t>Summer 2021</t>
   </si>
   <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>Opening</t>
+  </si>
+  <si>
+    <t>Ending</t>
+  </si>
+  <si>
+    <t>new Degree {</t>
+  </si>
+  <si>
+    <t>},</t>
+  </si>
+  <si>
+    <t>new Models.Requirement {</t>
+  </si>
+  <si>
     <t>opening</t>
   </si>
   <si>
     <t>ending</t>
   </si>
   <si>
-    <t>new Degree{</t>
-  </si>
-  <si>
-    <t>},</t>
-  </si>
-  <si>
-    <t>str</t>
-  </si>
-  <si>
-    <t>DegreeAbrrev</t>
-  </si>
-  <si>
-    <t>DegreeName</t>
-  </si>
-  <si>
-    <t>DegreeRequirementID</t>
-  </si>
-  <si>
-    <t>DegreePlanTermRequirementID</t>
-  </si>
-  <si>
-    <t>TermID</t>
-  </si>
-  <si>
-    <t>919(SID)</t>
-  </si>
-  <si>
-    <t>StudentTermID</t>
-  </si>
-  <si>
-    <t>TermLabel</t>
+    <t>new Models.DegreeRequirement {</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>new Model.DegreePlanTermRequirement{</t>
+  </si>
+  <si>
+    <t>DegreePlanAbbrev</t>
+  </si>
+  <si>
+    <t>DegreePlanName</t>
+  </si>
+  <si>
+    <t>new Model.DegreePlan{</t>
+  </si>
+  <si>
+    <t>new Model.Student{</t>
+  </si>
+  <si>
+    <t>new StudentTerm{</t>
   </si>
 </sst>
 </file>
@@ -325,9 +353,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,100 +644,122 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" t="s">
-        <v>72</v>
+        <v>80</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="F2" t="str">
-        <f>D2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"='"&amp;B2&amp;"','"&amp;$C$1&amp;"='"&amp;C2&amp;"'),"</f>
-        <v>new Degree{DegreeID=1,DegreeAbrrev='ACS+2','DegreeName='MS ACS +2 '),</v>
+        <f xml:space="preserve"> D2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;E2</f>
+        <v>new Degree {DegreeId=1,DegreeAbrrev(unique,max 6 characters)=ACS+2,DegreeName(unique, max 20 characters)=MS ACS +2 },</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="str">
+        <f xml:space="preserve"> D3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;E3</f>
+        <v>new Degree {DegreeId=2,DegreeAbrrev(unique,max 6 characters)=ACS+DB,DegreeName(unique, max 20 characters)=MS ACS +DB},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F5" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"='"&amp;B3&amp;"','"&amp;$C$1&amp;"='"&amp;C3&amp;"'),"</f>
-        <v>DegreeID=2,DegreeAbrrev='ACS+DB','DegreeName='MS ACS +DB'),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" t="str">
+        <f xml:space="preserve"> D4&amp;$A$1&amp;"="&amp;A4&amp;","&amp;$B$1&amp;"="&amp;B4&amp;","&amp;$C$1&amp;"="&amp;C4&amp;E4</f>
+        <v>new Degree {DegreeId=3,DegreeAbrrev(unique,max 6 characters)=ACS+NF,DegreeName(unique, max 20 characters)=MS ACS+NF},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="str">
-        <f t="shared" si="0"/>
-        <v>DegreeID=3,DegreeAbrrev='ACS+NF','DegreeName='MS ACS+NF'),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>DegreeID=4,DegreeAbrrev='ACS','DegreeName='MS ACS'),</v>
+        <f xml:space="preserve"> D5&amp;$A$1&amp;"="&amp;A5&amp;","&amp;$B$1&amp;"="&amp;B5&amp;","&amp;$C$1&amp;"="&amp;C5&amp;E5</f>
+        <v>new Degree {DegreeId=4,DegreeAbrrev(unique,max 6 characters)=ACS,DegreeName(unique, max 20 characters)=MS ACS},</v>
       </c>
     </row>
   </sheetData>
@@ -714,170 +770,313 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="137.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>460</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="str">
+        <f>D2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;E2</f>
+        <v>new Models.Requirement {RequirementID=460,RequirementAbbrev(unique,max 6)=DB,RequirementName(unique, max 20)=44-460 Database},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>356</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F14" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;E3</f>
+        <v>new Models.Requirement {RequirementID=356,RequirementAbbrev(unique,max 6)=NF,RequirementName(unique, max 20)=44-356 Network Fundamemtals},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>542</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.Requirement {RequirementID=542,RequirementAbbrev(unique,max 6)=OOP,RequirementName(unique, max 20)=44-542 OOP with Java},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>563</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.Requirement {RequirementID=563,RequirementAbbrev(unique,max 6)=Web apps,RequirementName(unique, max 20)=44-563 Web apps},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>560</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.Requirement {RequirementID=560,RequirementAbbrev(unique,max 6)=ADB,RequirementName(unique, max 20)=44-560 ADB},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>555</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.Requirement {RequirementID=555,RequirementAbbrev(unique,max 6)=NS,RequirementName(unique, max 20)=44-555 Network Security},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>618</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.Requirement {RequirementID=618,RequirementAbbrev(unique,max 6)=PM,RequirementName(unique, max 20)=44-618 PM},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.Requirement {RequirementID=1,RequirementAbbrev(unique,max 6)=Mobile,RequirementName(unique, max 20)=44-643 or 44-644},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>664</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.Requirement {RequirementID=664,RequirementAbbrev(unique,max 6)=UX,RequirementName(unique, max 20)=44-664 UX},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.Requirement {RequirementID=10,RequirementAbbrev(unique,max 6)=E1,RequirementName(unique, max 20)=Elective 1},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.Requirement {RequirementID=20,RequirementAbbrev(unique,max 6)=E2,RequirementName(unique, max 20)=Elective 2},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>691</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.Requirement {RequirementID=691,RequirementAbbrev(unique,max 6)=GDP1,RequirementName(unique, max 20)=GDP1},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>692</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.Requirement {RequirementID=692,RequirementAbbrev(unique,max 6)=GDP2,RequirementName(unique, max 20)=GDP2},</v>
       </c>
     </row>
   </sheetData>
@@ -887,31 +1086,41 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="6" max="6" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -921,8 +1130,18 @@
       <c r="C2">
         <v>460</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="str">
+        <f>D2&amp;$A$1&amp;"="&amp;A2&amp;""&amp;$B$1&amp;"="&amp;B2&amp;""&amp;$C$1&amp;"="""&amp;C2&amp;E2</f>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=1DegreeId=1RequirementId="460},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -932,8 +1151,18 @@
       <c r="C3">
         <v>356</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F49" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;E3</f>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=2,DegreeId=1,RequirementId=356},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -943,8 +1172,18 @@
       <c r="C4">
         <v>542</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=3,DegreeId=1,RequirementId=542},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -954,8 +1193,18 @@
       <c r="C5">
         <v>563</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=4,DegreeId=1,RequirementId=563},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -965,8 +1214,18 @@
       <c r="C6">
         <v>560</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=5,DegreeId=1,RequirementId=560},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -976,8 +1235,18 @@
       <c r="C7">
         <v>555</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=6,DegreeId=1,RequirementId=555},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -987,8 +1256,18 @@
       <c r="C8">
         <v>618</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=7,DegreeId=1,RequirementId=618},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -998,8 +1277,18 @@
       <c r="C9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=8,DegreeId=1,RequirementId=1},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1009,8 +1298,18 @@
       <c r="C10">
         <v>664</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=9,DegreeId=1,RequirementId=664},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1020,8 +1319,18 @@
       <c r="C11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=10,DegreeId=1,RequirementId=10},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1031,8 +1340,18 @@
       <c r="C12">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=11,DegreeId=1,RequirementId=20},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1042,8 +1361,18 @@
       <c r="C13">
         <v>691</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=12,DegreeId=1,RequirementId=691},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1053,8 +1382,18 @@
       <c r="C14">
         <v>692</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=13,DegreeId=1,RequirementId=692},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1064,8 +1403,18 @@
       <c r="C15">
         <v>460</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=14,DegreeId=2,RequirementId=460},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1075,8 +1424,18 @@
       <c r="C16">
         <v>542</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=15,DegreeId=2,RequirementId=542},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1086,8 +1445,18 @@
       <c r="C17">
         <v>563</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=16,DegreeId=2,RequirementId=563},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1097,8 +1466,18 @@
       <c r="C18">
         <v>560</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=17,DegreeId=2,RequirementId=560},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1108,8 +1487,18 @@
       <c r="C19">
         <v>555</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=18,DegreeId=2,RequirementId=555},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1119,8 +1508,18 @@
       <c r="C20">
         <v>618</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=19,DegreeId=2,RequirementId=618},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1130,8 +1529,18 @@
       <c r="C21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=20,DegreeId=2,RequirementId=1},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1141,8 +1550,18 @@
       <c r="C22">
         <v>664</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=21,DegreeId=2,RequirementId=664},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1152,8 +1571,18 @@
       <c r="C23">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" t="s">
+        <v>81</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=22,DegreeId=2,RequirementId=10},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1163,8 +1592,18 @@
       <c r="C24">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=23,DegreeId=2,RequirementId=20},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1174,8 +1613,18 @@
       <c r="C25">
         <v>691</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=24,DegreeId=2,RequirementId=691},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1185,8 +1634,18 @@
       <c r="C26">
         <v>692</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=25,DegreeId=2,RequirementId=692},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1196,8 +1655,18 @@
       <c r="C27">
         <v>356</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" t="s">
+        <v>81</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=26,DegreeId=3,RequirementId=356},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1207,8 +1676,18 @@
       <c r="C28">
         <v>542</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=27,DegreeId=3,RequirementId=542},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1218,8 +1697,18 @@
       <c r="C29">
         <v>563</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=28,DegreeId=3,RequirementId=563},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1229,8 +1718,18 @@
       <c r="C30">
         <v>560</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=29,DegreeId=3,RequirementId=560},</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1240,8 +1739,18 @@
       <c r="C31">
         <v>555</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=30,DegreeId=3,RequirementId=555},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1251,8 +1760,18 @@
       <c r="C32">
         <v>618</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=31,DegreeId=3,RequirementId=618},</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1262,8 +1781,18 @@
       <c r="C33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=32,DegreeId=3,RequirementId=1},</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1273,8 +1802,18 @@
       <c r="C34">
         <v>664</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" t="s">
+        <v>81</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=33,DegreeId=3,RequirementId=664},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1284,8 +1823,18 @@
       <c r="C35">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=34,DegreeId=3,RequirementId=10},</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1295,8 +1844,18 @@
       <c r="C36">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=35,DegreeId=3,RequirementId=20},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1306,8 +1865,18 @@
       <c r="C37">
         <v>691</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>85</v>
+      </c>
+      <c r="E37" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=36,DegreeId=3,RequirementId=691},</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1317,8 +1886,18 @@
       <c r="C38">
         <v>692</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>85</v>
+      </c>
+      <c r="E38" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=37,DegreeId=3,RequirementId=692},</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1328,8 +1907,18 @@
       <c r="C39">
         <v>542</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>85</v>
+      </c>
+      <c r="E39" t="s">
+        <v>81</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=38,DegreeId=4,RequirementId=542},</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1339,8 +1928,18 @@
       <c r="C40">
         <v>563</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>85</v>
+      </c>
+      <c r="E40" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=39,DegreeId=4,RequirementId=563},</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1350,8 +1949,18 @@
       <c r="C41">
         <v>560</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=40,DegreeId=4,RequirementId=560},</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1361,8 +1970,18 @@
       <c r="C42">
         <v>555</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>85</v>
+      </c>
+      <c r="E42" t="s">
+        <v>81</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=41,DegreeId=4,RequirementId=555},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1372,8 +1991,18 @@
       <c r="C43">
         <v>618</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>85</v>
+      </c>
+      <c r="E43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=42,DegreeId=4,RequirementId=618},</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1383,8 +2012,18 @@
       <c r="C44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" t="s">
+        <v>81</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=43,DegreeId=4,RequirementId=1},</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1394,8 +2033,18 @@
       <c r="C45">
         <v>664</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>85</v>
+      </c>
+      <c r="E45" t="s">
+        <v>81</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=44,DegreeId=4,RequirementId=664},</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1405,8 +2054,18 @@
       <c r="C46">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46" t="s">
+        <v>81</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=45,DegreeId=4,RequirementId=10},</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1416,8 +2075,18 @@
       <c r="C47">
         <v>20</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47" t="s">
+        <v>81</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=46,DegreeId=4,RequirementId=20},</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1427,8 +2096,18 @@
       <c r="C48">
         <v>691</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>85</v>
+      </c>
+      <c r="E48" t="s">
+        <v>81</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=47,DegreeId=4,RequirementId=691},</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1437,6 +2116,16 @@
       </c>
       <c r="C49">
         <v>692</v>
+      </c>
+      <c r="D49" t="s">
+        <v>85</v>
+      </c>
+      <c r="E49" t="s">
+        <v>81</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>new Models.DegreeRequirement {DegreeRequirementId=48,DegreeId=4,RequirementId=692},</v>
       </c>
     </row>
   </sheetData>
@@ -1446,34 +2135,43 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="F68" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1486,8 +2184,18 @@
       <c r="D2">
         <v>560</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" t="str">
+        <f>E2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"="&amp;D2&amp;F2</f>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=1,DegreePlanID=10,TermId=1,RequirementId=560},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1500,8 +2208,18 @@
       <c r="D3">
         <v>542</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G66" si="0">E3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;","&amp;$D$1&amp;"="&amp;D3&amp;F3</f>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=2,DegreePlanID=10,TermId=1,RequirementId=542},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1514,8 +2232,18 @@
       <c r="D4">
         <v>563</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=3,DegreePlanID=10,TermId=1,RequirementId=563},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1528,8 +2256,18 @@
       <c r="D5">
         <v>555</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=4,DegreePlanID=10,TermId=2,RequirementId=555},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1542,8 +2280,18 @@
       <c r="D6">
         <v>618</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=5,DegreePlanID=10,TermId=2,RequirementId=618},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1556,8 +2304,18 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=6,DegreePlanID=10,TermId=3,RequirementId=1},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1570,8 +2328,18 @@
       <c r="D8">
         <v>664</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=7,DegreePlanID=10,TermId=3,RequirementId=664},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1584,8 +2352,18 @@
       <c r="D9">
         <v>691</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=8,DegreePlanID=10,TermId=3,RequirementId=691},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1598,8 +2376,18 @@
       <c r="D10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=9,DegreePlanID=10,TermId=4,RequirementId=10},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1612,8 +2400,18 @@
       <c r="D11">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=10,DegreePlanID=10,TermId=4,RequirementId=20},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1626,8 +2424,18 @@
       <c r="D12">
         <v>692</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=11,DegreePlanID=10,TermId=5,RequirementId=692},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1640,8 +2448,18 @@
       <c r="D13">
         <v>560</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=12,DegreePlanID=11,TermId=1,RequirementId=560},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1654,8 +2472,18 @@
       <c r="D14">
         <v>542</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=13,DegreePlanID=11,TermId=1,RequirementId=542},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1668,8 +2496,18 @@
       <c r="D15">
         <v>563</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=14,DegreePlanID=11,TermId=1,RequirementId=563},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1682,8 +2520,18 @@
       <c r="D16">
         <v>555</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=15,DegreePlanID=11,TermId=2,RequirementId=555},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1696,8 +2544,18 @@
       <c r="D17">
         <v>618</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=16,DegreePlanID=11,TermId=2,RequirementId=618},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1710,8 +2568,18 @@
       <c r="D18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=17,DegreePlanID=11,TermId=2,RequirementId=1},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1724,8 +2592,18 @@
       <c r="D19">
         <v>664</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=18,DegreePlanID=11,TermId=4,RequirementId=664},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1738,8 +2616,18 @@
       <c r="D20">
         <v>691</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=19,DegreePlanID=11,TermId=4,RequirementId=691},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1752,8 +2640,18 @@
       <c r="D21">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" t="s">
+        <v>81</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=20,DegreePlanID=11,TermId=4,RequirementId=10},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1766,8 +2664,18 @@
       <c r="D22">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=21,DegreePlanID=11,TermId=5,RequirementId=20},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1780,8 +2688,18 @@
       <c r="D23">
         <v>692</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=22,DegreePlanID=11,TermId=5,RequirementId=692},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1794,8 +2712,18 @@
       <c r="D24">
         <v>560</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=23,DegreePlanID=12,TermId=1,RequirementId=560},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1808,8 +2736,18 @@
       <c r="D25">
         <v>542</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=24,DegreePlanID=12,TermId=1,RequirementId=542},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1822,8 +2760,18 @@
       <c r="D26">
         <v>563</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=25,DegreePlanID=12,TermId=1,RequirementId=563},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1836,8 +2784,18 @@
       <c r="D27">
         <v>555</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=26,DegreePlanID=12,TermId=2,RequirementId=555},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1850,8 +2808,18 @@
       <c r="D28">
         <v>618</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" t="s">
+        <v>81</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=27,DegreePlanID=12,TermId=2,RequirementId=618},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1864,8 +2832,18 @@
       <c r="D29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=28,DegreePlanID=12,TermId=3,RequirementId=1},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1878,8 +2856,18 @@
       <c r="D30">
         <v>664</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>87</v>
+      </c>
+      <c r="F30" t="s">
+        <v>81</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=29,DegreePlanID=12,TermId=3,RequirementId=664},</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1892,8 +2880,18 @@
       <c r="D31">
         <v>691</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" t="s">
+        <v>81</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=30,DegreePlanID=12,TermId=3,RequirementId=691},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1906,8 +2904,18 @@
       <c r="D32">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>87</v>
+      </c>
+      <c r="F32" t="s">
+        <v>81</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=31,DegreePlanID=12,TermId=4,RequirementId=10},</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1920,8 +2928,18 @@
       <c r="D33">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>87</v>
+      </c>
+      <c r="F33" t="s">
+        <v>81</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=32,DegreePlanID=12,TermId=4,RequirementId=20},</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1934,8 +2952,18 @@
       <c r="D34">
         <v>692</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>87</v>
+      </c>
+      <c r="F34" t="s">
+        <v>81</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=33,DegreePlanID=12,TermId=5,RequirementId=692},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1948,8 +2976,18 @@
       <c r="D35">
         <v>560</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>87</v>
+      </c>
+      <c r="F35" t="s">
+        <v>81</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=34,DegreePlanID=13,TermId=1,RequirementId=560},</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1962,8 +3000,18 @@
       <c r="D36">
         <v>542</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>87</v>
+      </c>
+      <c r="F36" t="s">
+        <v>81</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=35,DegreePlanID=13,TermId=1,RequirementId=542},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1976,8 +3024,18 @@
       <c r="D37">
         <v>563</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>87</v>
+      </c>
+      <c r="F37" t="s">
+        <v>81</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=36,DegreePlanID=13,TermId=1,RequirementId=563},</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1990,8 +3048,18 @@
       <c r="D38">
         <v>555</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>87</v>
+      </c>
+      <c r="F38" t="s">
+        <v>81</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=37,DegreePlanID=13,TermId=3,RequirementId=555},</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2004,8 +3072,18 @@
       <c r="D39">
         <v>618</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>87</v>
+      </c>
+      <c r="F39" t="s">
+        <v>81</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=38,DegreePlanID=13,TermId=3,RequirementId=618},</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2018,8 +3096,18 @@
       <c r="D40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>87</v>
+      </c>
+      <c r="F40" t="s">
+        <v>81</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=39,DegreePlanID=13,TermId=3,RequirementId=1},</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2032,8 +3120,18 @@
       <c r="D41">
         <v>664</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>87</v>
+      </c>
+      <c r="F41" t="s">
+        <v>81</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=40,DegreePlanID=13,TermId=4,RequirementId=664},</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2046,8 +3144,18 @@
       <c r="D42">
         <v>691</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>87</v>
+      </c>
+      <c r="F42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=41,DegreePlanID=13,TermId=4,RequirementId=691},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2060,8 +3168,18 @@
       <c r="D43">
         <v>10</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>87</v>
+      </c>
+      <c r="F43" t="s">
+        <v>81</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=42,DegreePlanID=13,TermId=4,RequirementId=10},</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2074,8 +3192,18 @@
       <c r="D44">
         <v>20</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>87</v>
+      </c>
+      <c r="F44" t="s">
+        <v>81</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=43,DegreePlanID=13,TermId=5,RequirementId=20},</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2088,8 +3216,18 @@
       <c r="D45">
         <v>692</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>87</v>
+      </c>
+      <c r="F45" t="s">
+        <v>81</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=44,DegreePlanID=13,TermId=5,RequirementId=692},</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2102,8 +3240,18 @@
       <c r="D46">
         <v>560</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>87</v>
+      </c>
+      <c r="F46" t="s">
+        <v>81</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=45,DegreePlanID=14,TermId=1,RequirementId=560},</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2116,8 +3264,18 @@
       <c r="D47">
         <v>542</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>87</v>
+      </c>
+      <c r="F47" t="s">
+        <v>81</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=46,DegreePlanID=14,TermId=1,RequirementId=542},</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2130,8 +3288,18 @@
       <c r="D48">
         <v>563</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>87</v>
+      </c>
+      <c r="F48" t="s">
+        <v>81</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=47,DegreePlanID=14,TermId=1,RequirementId=563},</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2144,8 +3312,18 @@
       <c r="D49">
         <v>555</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>87</v>
+      </c>
+      <c r="F49" t="s">
+        <v>81</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=48,DegreePlanID=14,TermId=2,RequirementId=555},</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2158,8 +3336,18 @@
       <c r="D50">
         <v>618</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>87</v>
+      </c>
+      <c r="F50" t="s">
+        <v>81</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=49,DegreePlanID=14,TermId=2,RequirementId=618},</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2172,8 +3360,18 @@
       <c r="D51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>87</v>
+      </c>
+      <c r="F51" t="s">
+        <v>81</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=50,DegreePlanID=14,TermId=3,RequirementId=1},</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2186,8 +3384,18 @@
       <c r="D52">
         <v>664</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>87</v>
+      </c>
+      <c r="F52" t="s">
+        <v>81</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=51,DegreePlanID=14,TermId=3,RequirementId=664},</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2200,8 +3408,18 @@
       <c r="D53">
         <v>691</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>87</v>
+      </c>
+      <c r="F53" t="s">
+        <v>81</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=52,DegreePlanID=14,TermId=3,RequirementId=691},</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2214,8 +3432,18 @@
       <c r="D54">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>87</v>
+      </c>
+      <c r="F54" t="s">
+        <v>81</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=53,DegreePlanID=14,TermId=4,RequirementId=10},</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2228,8 +3456,18 @@
       <c r="D55">
         <v>20</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>87</v>
+      </c>
+      <c r="F55" t="s">
+        <v>81</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=54,DegreePlanID=14,TermId=4,RequirementId=20},</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2242,8 +3480,18 @@
       <c r="D56">
         <v>692</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>87</v>
+      </c>
+      <c r="F56" t="s">
+        <v>81</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=55,DegreePlanID=14,TermId=5,RequirementId=692},</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2256,8 +3504,18 @@
       <c r="D57">
         <v>560</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>87</v>
+      </c>
+      <c r="F57" t="s">
+        <v>81</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=56,DegreePlanID=15,TermId=1,RequirementId=560},</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2270,8 +3528,18 @@
       <c r="D58">
         <v>542</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
+        <v>87</v>
+      </c>
+      <c r="F58" t="s">
+        <v>81</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=57,DegreePlanID=15,TermId=1,RequirementId=542},</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2284,8 +3552,18 @@
       <c r="D59">
         <v>563</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>87</v>
+      </c>
+      <c r="F59" t="s">
+        <v>81</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=58,DegreePlanID=15,TermId=1,RequirementId=563},</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2298,8 +3576,18 @@
       <c r="D60">
         <v>555</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>87</v>
+      </c>
+      <c r="F60" t="s">
+        <v>81</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=59,DegreePlanID=15,TermId=2,RequirementId=555},</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2312,8 +3600,18 @@
       <c r="D61">
         <v>618</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>87</v>
+      </c>
+      <c r="F61" t="s">
+        <v>81</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=60,DegreePlanID=15,TermId=2,RequirementId=618},</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2326,8 +3624,18 @@
       <c r="D62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>87</v>
+      </c>
+      <c r="F62" t="s">
+        <v>81</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=61,DegreePlanID=15,TermId=2,RequirementId=1},</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2340,8 +3648,18 @@
       <c r="D63">
         <v>664</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>87</v>
+      </c>
+      <c r="F63" t="s">
+        <v>81</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=62,DegreePlanID=15,TermId=4,RequirementId=664},</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2354,8 +3672,18 @@
       <c r="D64">
         <v>691</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>87</v>
+      </c>
+      <c r="F64" t="s">
+        <v>81</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=63,DegreePlanID=15,TermId=4,RequirementId=691},</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2368,8 +3696,18 @@
       <c r="D65">
         <v>10</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>87</v>
+      </c>
+      <c r="F65" t="s">
+        <v>81</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=64,DegreePlanID=15,TermId=4,RequirementId=10},</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2382,8 +3720,18 @@
       <c r="D66">
         <v>20</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>87</v>
+      </c>
+      <c r="F66" t="s">
+        <v>81</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=65,DegreePlanID=15,TermId=5,RequirementId=20},</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2396,8 +3744,18 @@
       <c r="D67">
         <v>692</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>87</v>
+      </c>
+      <c r="F67" t="s">
+        <v>81</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" ref="G67:G89" si="1">E67&amp;$A$1&amp;"="&amp;A67&amp;","&amp;$B$1&amp;"="&amp;B67&amp;","&amp;$C$1&amp;"="&amp;C67&amp;","&amp;$D$1&amp;"="&amp;D67&amp;F67</f>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=66,DegreePlanID=15,TermId=5,RequirementId=692},</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2410,8 +3768,18 @@
       <c r="D68">
         <v>560</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>87</v>
+      </c>
+      <c r="F68" t="s">
+        <v>81</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=67,DegreePlanID=16,TermId=1,RequirementId=560},</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2424,8 +3792,18 @@
       <c r="D69">
         <v>542</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
+        <v>87</v>
+      </c>
+      <c r="F69" t="s">
+        <v>81</v>
+      </c>
+      <c r="G69" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=68,DegreePlanID=16,TermId=1,RequirementId=542},</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2438,8 +3816,18 @@
       <c r="D70">
         <v>563</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" t="s">
+        <v>87</v>
+      </c>
+      <c r="F70" t="s">
+        <v>81</v>
+      </c>
+      <c r="G70" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=69,DegreePlanID=16,TermId=1,RequirementId=563},</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2452,8 +3840,18 @@
       <c r="D71">
         <v>555</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>87</v>
+      </c>
+      <c r="F71" t="s">
+        <v>81</v>
+      </c>
+      <c r="G71" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=70,DegreePlanID=16,TermId=2,RequirementId=555},</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2466,8 +3864,18 @@
       <c r="D72">
         <v>618</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" t="s">
+        <v>87</v>
+      </c>
+      <c r="F72" t="s">
+        <v>81</v>
+      </c>
+      <c r="G72" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=71,DegreePlanID=16,TermId=2,RequirementId=618},</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2480,8 +3888,18 @@
       <c r="D73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
+        <v>87</v>
+      </c>
+      <c r="F73" t="s">
+        <v>81</v>
+      </c>
+      <c r="G73" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=72,DegreePlanID=16,TermId=3,RequirementId=1},</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2494,8 +3912,18 @@
       <c r="D74">
         <v>664</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
+        <v>87</v>
+      </c>
+      <c r="F74" t="s">
+        <v>81</v>
+      </c>
+      <c r="G74" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=73,DegreePlanID=16,TermId=3,RequirementId=664},</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2508,8 +3936,18 @@
       <c r="D75">
         <v>691</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" t="s">
+        <v>87</v>
+      </c>
+      <c r="F75" t="s">
+        <v>81</v>
+      </c>
+      <c r="G75" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=74,DegreePlanID=16,TermId=4,RequirementId=691},</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2522,8 +3960,18 @@
       <c r="D76">
         <v>10</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
+        <v>87</v>
+      </c>
+      <c r="F76" t="s">
+        <v>81</v>
+      </c>
+      <c r="G76" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=75,DegreePlanID=16,TermId=4,RequirementId=10},</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2536,8 +3984,18 @@
       <c r="D77">
         <v>20</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
+        <v>87</v>
+      </c>
+      <c r="F77" t="s">
+        <v>81</v>
+      </c>
+      <c r="G77" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=76,DegreePlanID=16,TermId=4,RequirementId=20},</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2550,8 +4008,18 @@
       <c r="D78">
         <v>692</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>87</v>
+      </c>
+      <c r="F78" t="s">
+        <v>81</v>
+      </c>
+      <c r="G78" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=77,DegreePlanID=16,TermId=5,RequirementId=692},</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2564,8 +4032,18 @@
       <c r="D79">
         <v>560</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
+        <v>87</v>
+      </c>
+      <c r="F79" t="s">
+        <v>81</v>
+      </c>
+      <c r="G79" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=78,DegreePlanID=17,TermId=1,RequirementId=560},</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2578,8 +4056,18 @@
       <c r="D80">
         <v>542</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
+        <v>87</v>
+      </c>
+      <c r="F80" t="s">
+        <v>81</v>
+      </c>
+      <c r="G80" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=79,DegreePlanID=17,TermId=1,RequirementId=542},</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2592,8 +4080,18 @@
       <c r="D81">
         <v>563</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" t="s">
+        <v>87</v>
+      </c>
+      <c r="F81" t="s">
+        <v>81</v>
+      </c>
+      <c r="G81" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=80,DegreePlanID=17,TermId=1,RequirementId=563},</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2606,8 +4104,18 @@
       <c r="D82">
         <v>555</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
+        <v>87</v>
+      </c>
+      <c r="F82" t="s">
+        <v>81</v>
+      </c>
+      <c r="G82" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=81,DegreePlanID=17,TermId=3,RequirementId=555},</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2620,8 +4128,18 @@
       <c r="D83">
         <v>618</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
+        <v>87</v>
+      </c>
+      <c r="F83" t="s">
+        <v>81</v>
+      </c>
+      <c r="G83" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=82,DegreePlanID=17,TermId=3,RequirementId=618},</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2634,8 +4152,18 @@
       <c r="D84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" t="s">
+        <v>87</v>
+      </c>
+      <c r="F84" t="s">
+        <v>81</v>
+      </c>
+      <c r="G84" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=83,DegreePlanID=17,TermId=3,RequirementId=1},</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2648,8 +4176,18 @@
       <c r="D85">
         <v>664</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" t="s">
+        <v>87</v>
+      </c>
+      <c r="F85" t="s">
+        <v>81</v>
+      </c>
+      <c r="G85" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=84,DegreePlanID=17,TermId=4,RequirementId=664},</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2662,8 +4200,18 @@
       <c r="D86">
         <v>691</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
+        <v>87</v>
+      </c>
+      <c r="F86" t="s">
+        <v>81</v>
+      </c>
+      <c r="G86" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=85,DegreePlanID=17,TermId=4,RequirementId=691},</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2676,8 +4224,18 @@
       <c r="D87">
         <v>10</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" t="s">
+        <v>87</v>
+      </c>
+      <c r="F87" t="s">
+        <v>81</v>
+      </c>
+      <c r="G87" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=86,DegreePlanID=17,TermId=4,RequirementId=10},</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2690,8 +4248,18 @@
       <c r="D88">
         <v>20</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" t="s">
+        <v>87</v>
+      </c>
+      <c r="F88" t="s">
+        <v>81</v>
+      </c>
+      <c r="G88" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=87,DegreePlanID=17,TermId=5,RequirementId=20},</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2703,6 +4271,16 @@
       </c>
       <c r="D89">
         <v>692</v>
+      </c>
+      <c r="E89" t="s">
+        <v>87</v>
+      </c>
+      <c r="F89" t="s">
+        <v>81</v>
+      </c>
+      <c r="G89" t="str">
+        <f t="shared" si="1"/>
+        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=88,DegreePlanID=17,TermId=5,RequirementId=692},</v>
       </c>
     </row>
   </sheetData>
@@ -2712,37 +4290,47 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H2" sqref="H2:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="3" width="24.42578125" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="F1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -2753,13 +4341,23 @@
         <v>531441</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" t="str">
+        <f>F2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"="&amp;D2&amp;","&amp;$E$1&amp;"="&amp;E2&amp;G2</f>
+        <v>new Model.DegreePlan{DegreePlanId=10,DegreeID=4,StudentId=531441,DegreePlanAbbrev=No summer off,DegreePlanName=As Fast as I Can},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11</v>
       </c>
@@ -2770,13 +4368,23 @@
         <v>531441</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H9" si="0">F3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;","&amp;$D$1&amp;"="&amp;D3&amp;","&amp;$E$1&amp;"="&amp;E3&amp;G3</f>
+        <v>new Model.DegreePlan{DegreePlanId=11,DegreeID=4,StudentId=531441,DegreePlanAbbrev=Summer Off,DegreePlanName=Slow and Easy},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12</v>
       </c>
@@ -2787,13 +4395,23 @@
         <v>531524</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlan{DegreePlanId=12,DegreeID=4,StudentId=531524,DegreePlanAbbrev=No summer off,DegreePlanName=As Fast as I Can},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13</v>
       </c>
@@ -2804,13 +4422,23 @@
         <v>531524</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlan{DegreePlanId=13,DegreeID=4,StudentId=531524,DegreePlanAbbrev=Summer Off,DegreePlanName=Slow and Easy},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>14</v>
       </c>
@@ -2821,13 +4449,23 @@
         <v>531506</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlan{DegreePlanId=14,DegreeID=4,StudentId=531506,DegreePlanAbbrev=No summer off,DegreePlanName=As Fast as I Can},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>15</v>
       </c>
@@ -2838,13 +4476,23 @@
         <v>531506</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlan{DegreePlanId=15,DegreeID=4,StudentId=531506,DegreePlanAbbrev=Summer Off,DegreePlanName=Slow and Easy},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>16</v>
       </c>
@@ -2855,13 +4503,23 @@
         <v>530469</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlan{DegreePlanId=16,DegreeID=4,StudentId=530469,DegreePlanAbbrev=No summer off,DegreePlanName=As Fast as I Can},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>17</v>
       </c>
@@ -2872,10 +4530,20 @@
         <v>530469</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.DegreePlan{DegreePlanId=17,DegreeID=4,StudentId=530469,DegreePlanAbbrev=Summer Off,DegreePlanName=Slow and Easy},</v>
       </c>
     </row>
   </sheetData>
@@ -2885,43 +4553,52 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="E1">
+        <v>919</v>
+      </c>
+      <c r="F1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>531441</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D2">
         <v>531441</v>
@@ -2929,16 +4606,26 @@
       <c r="E2">
         <v>919562404</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" t="str">
+        <f>F2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"="&amp;D2&amp;","&amp;$E$1&amp;"="&amp;E2&amp;G2</f>
+        <v>new Model.Student{StudentId=531441,First=Vyshnavi srilaxmi ,Last=Thannir,Snumber=531441,919=919562404},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>531524</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D3">
         <v>531524</v>
@@ -2946,16 +4633,26 @@
       <c r="E3">
         <v>919562444</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H5" si="0">F3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;","&amp;$D$1&amp;"="&amp;D3&amp;","&amp;$E$1&amp;"="&amp;E3&amp;G3</f>
+        <v>new Model.Student{StudentId=531524,First=Sri Ram Teja,Last=Komerisetti,Snumber=531524,919=919562444},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>530469</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D4">
         <v>530469</v>
@@ -2963,22 +4660,42 @@
       <c r="E4">
         <v>919559547</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.Student{StudentId=530469,First=Chandra Mouli,Last=Kantipudi,Snumber=530469,919=919559547},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>531506</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D5">
         <v>531506</v>
       </c>
       <c r="E5">
         <v>919562179</v>
+      </c>
+      <c r="F5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>new Model.Student{StudentId=531506,First=Prashanth Kumar,Last=Thallada,Snumber=531506,919=919562179},</v>
       </c>
     </row>
   </sheetData>
@@ -2988,32 +4705,42 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3024,10 +4751,20 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" t="str">
+        <f>E2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"="&amp;D2&amp;F2</f>
+        <v>new StudentTerm{StudentTermId=1,StudentID=531441,Term=1,Term Label=Fall 2017},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3038,10 +4775,20 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G21" si="0">E3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;","&amp;$D$1&amp;"="&amp;D3&amp;F3</f>
+        <v>new StudentTerm{StudentTermId=2,StudentID=531441,Term=2,Term Label=Spring 2018},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3052,10 +4799,20 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=3,StudentID=531441,Term=3,Term Label=Summer 2018},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3066,10 +4823,20 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=4,StudentID=531441,Term=4,Term Label=Fall 2018},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3080,10 +4847,20 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="E6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=5,StudentID=531441,Term=5,Term Label=Spring 2019},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3094,10 +4871,20 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=6,StudentID=531524,Term=1,Term Label=Spring 2018},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3108,10 +4895,20 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="E8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=7,StudentID=531524,Term=2,Term Label=Summer 2018},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3122,10 +4919,20 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="E9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=8,StudentID=531524,Term=3,Term Label=Fall 2018},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3136,10 +4943,20 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=9,StudentID=531524,Term=4,Term Label=Spring 2019},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3150,10 +4967,20 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=10,StudentID=531524,Term=5,Term Label=Summer 2019},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3164,10 +4991,20 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=11,StudentID=530469,Term=1,Term Label=Fall 2018},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3178,10 +5015,20 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="E13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=12,StudentID=530469,Term=2,Term Label=Spring 2019},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3192,10 +5039,20 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=13,StudentID=530469,Term=3,Term Label=Summer 2019},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3206,10 +5063,20 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="E15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=14,StudentID=530469,Term=4,Term Label=Fall 2019},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3220,10 +5087,20 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="E16" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=15,StudentID=530469,Term=5,Term Label=Spring 2020},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3234,10 +5111,20 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="E17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=16,StudentID=531506,Term=1,Term Label=Spring 2020},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3248,10 +5135,20 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=17,StudentID=531506,Term=2,Term Label=Summer 2020},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3262,10 +5159,20 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="E19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=18,StudentID=531506,Term=3,Term Label=Fall 2020},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3276,10 +5183,20 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="E20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=19,StudentID=531506,Term=4,Term Label=Spring 2021},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3290,7 +5207,17 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>76</v>
+      </c>
+      <c r="E21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" t="s">
+        <v>81</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm{StudentTermId=20,StudentID=531506,Term=5,Term Label=Summer 2021},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes to DBInitializer.cs
</commit_message>
<xml_diff>
--- a/MVC excel Assig.xlsx
+++ b/MVC excel Assig.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="90">
   <si>
     <t>DegreeId</t>
   </si>
@@ -147,30 +147,12 @@
     <t>GDP2</t>
   </si>
   <si>
-    <t>DegreeRequirementId</t>
-  </si>
-  <si>
-    <t>RequirementId</t>
-  </si>
-  <si>
-    <t>DegreePlanTermRequirementId</t>
-  </si>
-  <si>
     <t>DegreePlanID</t>
   </si>
   <si>
-    <t>TermId</t>
-  </si>
-  <si>
-    <t>DegreePlanId</t>
-  </si>
-  <si>
     <t>DegreeID</t>
   </si>
   <si>
-    <t>StudentId</t>
-  </si>
-  <si>
     <t>No summer off</t>
   </si>
   <si>
@@ -216,18 +198,9 @@
     <t>Thallada</t>
   </si>
   <si>
-    <t>StudentTermId</t>
-  </si>
-  <si>
     <t>StudentID</t>
   </si>
   <si>
-    <t>Term</t>
-  </si>
-  <si>
-    <t>Term Label</t>
-  </si>
-  <si>
     <t>Fall 2017</t>
   </si>
   <si>
@@ -294,22 +267,40 @@
     <t>end</t>
   </si>
   <si>
-    <t>new Model.DegreePlanTermRequirement{</t>
-  </si>
-  <si>
     <t>DegreePlanAbbrev</t>
   </si>
   <si>
     <t>DegreePlanName</t>
   </si>
   <si>
-    <t>new Model.DegreePlan{</t>
-  </si>
-  <si>
-    <t>new Model.Student{</t>
-  </si>
-  <si>
-    <t>new StudentTerm{</t>
+    <t>new Models.DegreePlanTermRequirement{</t>
+  </si>
+  <si>
+    <t>new Models.DegreePlan{</t>
+  </si>
+  <si>
+    <t>new Models.Student{</t>
+  </si>
+  <si>
+    <t>new Models.StudentTerm{</t>
+  </si>
+  <si>
+    <t>DegreeRequirementID</t>
+  </si>
+  <si>
+    <t>DegreePlanTermRequirementID</t>
+  </si>
+  <si>
+    <t>TermID</t>
+  </si>
+  <si>
+    <t>SID</t>
+  </si>
+  <si>
+    <t>StudentTermID</t>
+  </si>
+  <si>
+    <t>TermLabel</t>
   </si>
 </sst>
 </file>
@@ -669,13 +660,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -689,10 +680,10 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F2" t="str">
         <f xml:space="preserve"> D2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;E2</f>
@@ -710,10 +701,10 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F3" t="str">
         <f xml:space="preserve"> D3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;E3</f>
@@ -731,10 +722,10 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F4" t="str">
         <f xml:space="preserve"> D4&amp;$A$1&amp;"="&amp;A4&amp;","&amp;$B$1&amp;"="&amp;B4&amp;","&amp;$C$1&amp;"="&amp;C4&amp;E4</f>
@@ -752,10 +743,10 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F5" t="str">
         <f xml:space="preserve"> D5&amp;$A$1&amp;"="&amp;A5&amp;","&amp;$B$1&amp;"="&amp;B5&amp;","&amp;$C$1&amp;"="&amp;C5&amp;E5</f>
@@ -797,13 +788,13 @@
         <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -817,10 +808,10 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F2" t="str">
         <f>D2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;E2</f>
@@ -838,10 +829,10 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F14" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;E3</f>
@@ -859,10 +850,10 @@
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -880,10 +871,10 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -901,10 +892,10 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -922,10 +913,10 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -943,10 +934,10 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
@@ -964,10 +955,10 @@
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
@@ -985,10 +976,10 @@
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -1006,10 +997,10 @@
         <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
@@ -1027,10 +1018,10 @@
         <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
@@ -1048,10 +1039,10 @@
         <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
@@ -1069,10 +1060,10 @@
         <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
@@ -1088,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="C33" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,22 +1093,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1131,14 +1122,14 @@
         <v>460</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F2" t="str">
-        <f>D2&amp;$A$1&amp;"="&amp;A2&amp;""&amp;$B$1&amp;"="&amp;B2&amp;""&amp;$C$1&amp;"="""&amp;C2&amp;E2</f>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=1DegreeId=1RequirementId="460},</v>
+        <f>D2&amp;$A$1&amp;"="&amp;A2&amp;""&amp;$B$1&amp;"="&amp;B2&amp;""&amp;$C$1&amp;"="&amp;C2&amp;E2</f>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=1DegreeID=1RequirementID=460},</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1152,14 +1143,14 @@
         <v>356</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F49" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;E3</f>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=2,DegreeId=1,RequirementId=356},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=2,DegreeID=1,RequirementID=356},</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1173,14 +1164,14 @@
         <v>542</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=3,DegreeId=1,RequirementId=542},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=3,DegreeID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1194,14 +1185,14 @@
         <v>563</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=4,DegreeId=1,RequirementId=563},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=4,DegreeID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1215,14 +1206,14 @@
         <v>560</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=5,DegreeId=1,RequirementId=560},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=5,DegreeID=1,RequirementID=560},</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1236,14 +1227,14 @@
         <v>555</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=6,DegreeId=1,RequirementId=555},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=6,DegreeID=1,RequirementID=555},</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1257,14 +1248,14 @@
         <v>618</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=7,DegreeId=1,RequirementId=618},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=7,DegreeID=1,RequirementID=618},</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1278,14 +1269,14 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=8,DegreeId=1,RequirementId=1},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=8,DegreeID=1,RequirementID=1},</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1299,14 +1290,14 @@
         <v>664</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=9,DegreeId=1,RequirementId=664},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=9,DegreeID=1,RequirementID=664},</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1320,14 +1311,14 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=10,DegreeId=1,RequirementId=10},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=10,DegreeID=1,RequirementID=10},</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1341,14 +1332,14 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=11,DegreeId=1,RequirementId=20},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=11,DegreeID=1,RequirementID=20},</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1362,14 +1353,14 @@
         <v>691</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=12,DegreeId=1,RequirementId=691},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=12,DegreeID=1,RequirementID=691},</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1383,14 +1374,14 @@
         <v>692</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=13,DegreeId=1,RequirementId=692},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=13,DegreeID=1,RequirementID=692},</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1404,14 +1395,14 @@
         <v>460</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=14,DegreeId=2,RequirementId=460},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=14,DegreeID=2,RequirementID=460},</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1425,14 +1416,14 @@
         <v>542</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E16" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=15,DegreeId=2,RequirementId=542},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=15,DegreeID=2,RequirementID=542},</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1446,14 +1437,14 @@
         <v>563</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=16,DegreeId=2,RequirementId=563},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=16,DegreeID=2,RequirementID=563},</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1467,14 +1458,14 @@
         <v>560</v>
       </c>
       <c r="D18" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=17,DegreeId=2,RequirementId=560},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=17,DegreeID=2,RequirementID=560},</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1488,14 +1479,14 @@
         <v>555</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E19" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=18,DegreeId=2,RequirementId=555},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=18,DegreeID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1509,14 +1500,14 @@
         <v>618</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E20" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=19,DegreeId=2,RequirementId=618},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=19,DegreeID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1530,14 +1521,14 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E21" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=20,DegreeId=2,RequirementId=1},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=20,DegreeID=2,RequirementID=1},</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1551,14 +1542,14 @@
         <v>664</v>
       </c>
       <c r="D22" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=21,DegreeId=2,RequirementId=664},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=21,DegreeID=2,RequirementID=664},</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1572,14 +1563,14 @@
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E23" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=22,DegreeId=2,RequirementId=10},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=22,DegreeID=2,RequirementID=10},</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1593,14 +1584,14 @@
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E24" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=23,DegreeId=2,RequirementId=20},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=23,DegreeID=2,RequirementID=20},</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1614,14 +1605,14 @@
         <v>691</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E25" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=24,DegreeId=2,RequirementId=691},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=24,DegreeID=2,RequirementID=691},</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1635,14 +1626,14 @@
         <v>692</v>
       </c>
       <c r="D26" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E26" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=25,DegreeId=2,RequirementId=692},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=25,DegreeID=2,RequirementID=692},</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1656,14 +1647,14 @@
         <v>356</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=26,DegreeId=3,RequirementId=356},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=26,DegreeID=3,RequirementID=356},</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1677,14 +1668,14 @@
         <v>542</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E28" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=27,DegreeId=3,RequirementId=542},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=27,DegreeID=3,RequirementID=542},</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1698,14 +1689,14 @@
         <v>563</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E29" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=28,DegreeId=3,RequirementId=563},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=28,DegreeID=3,RequirementID=563},</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1719,14 +1710,14 @@
         <v>560</v>
       </c>
       <c r="D30" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E30" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=29,DegreeId=3,RequirementId=560},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=29,DegreeID=3,RequirementID=560},</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1740,14 +1731,14 @@
         <v>555</v>
       </c>
       <c r="D31" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E31" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=30,DegreeId=3,RequirementId=555},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=30,DegreeID=3,RequirementID=555},</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1761,14 +1752,14 @@
         <v>618</v>
       </c>
       <c r="D32" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E32" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=31,DegreeId=3,RequirementId=618},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=31,DegreeID=3,RequirementID=618},</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1782,14 +1773,14 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E33" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=32,DegreeId=3,RequirementId=1},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=32,DegreeID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1803,14 +1794,14 @@
         <v>664</v>
       </c>
       <c r="D34" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E34" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=33,DegreeId=3,RequirementId=664},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=33,DegreeID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1824,14 +1815,14 @@
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E35" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=34,DegreeId=3,RequirementId=10},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=34,DegreeID=3,RequirementID=10},</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1845,14 +1836,14 @@
         <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E36" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=35,DegreeId=3,RequirementId=20},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=35,DegreeID=3,RequirementID=20},</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1866,14 +1857,14 @@
         <v>691</v>
       </c>
       <c r="D37" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E37" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=36,DegreeId=3,RequirementId=691},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=36,DegreeID=3,RequirementID=691},</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1887,14 +1878,14 @@
         <v>692</v>
       </c>
       <c r="D38" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E38" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=37,DegreeId=3,RequirementId=692},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=37,DegreeID=3,RequirementID=692},</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1908,14 +1899,14 @@
         <v>542</v>
       </c>
       <c r="D39" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E39" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=38,DegreeId=4,RequirementId=542},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=38,DegreeID=4,RequirementID=542},</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1929,14 +1920,14 @@
         <v>563</v>
       </c>
       <c r="D40" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E40" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=39,DegreeId=4,RequirementId=563},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=39,DegreeID=4,RequirementID=563},</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1950,14 +1941,14 @@
         <v>560</v>
       </c>
       <c r="D41" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E41" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=40,DegreeId=4,RequirementId=560},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=40,DegreeID=4,RequirementID=560},</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1971,14 +1962,14 @@
         <v>555</v>
       </c>
       <c r="D42" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E42" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=41,DegreeId=4,RequirementId=555},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=41,DegreeID=4,RequirementID=555},</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1992,14 +1983,14 @@
         <v>618</v>
       </c>
       <c r="D43" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E43" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=42,DegreeId=4,RequirementId=618},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=42,DegreeID=4,RequirementID=618},</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2013,14 +2004,14 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E44" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=43,DegreeId=4,RequirementId=1},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=43,DegreeID=4,RequirementID=1},</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2034,14 +2025,14 @@
         <v>664</v>
       </c>
       <c r="D45" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E45" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=44,DegreeId=4,RequirementId=664},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=44,DegreeID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2055,14 +2046,14 @@
         <v>10</v>
       </c>
       <c r="D46" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E46" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=45,DegreeId=4,RequirementId=10},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=45,DegreeID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2076,14 +2067,14 @@
         <v>20</v>
       </c>
       <c r="D47" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E47" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=46,DegreeId=4,RequirementId=20},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=46,DegreeID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2097,14 +2088,14 @@
         <v>691</v>
       </c>
       <c r="D48" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E48" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=47,DegreeId=4,RequirementId=691},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=47,DegreeID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2118,14 +2109,14 @@
         <v>692</v>
       </c>
       <c r="D49" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E49" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
-        <v>new Models.DegreeRequirement {DegreeRequirementId=48,DegreeId=4,RequirementId=692},</v>
+        <v>new Models.DegreeRequirement {DegreeRequirementID=48,DegreeID=4,RequirementID=692},</v>
       </c>
     </row>
   </sheetData>
@@ -2137,38 +2128,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView topLeftCell="F68" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2185,14 +2177,14 @@
         <v>560</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G2" t="str">
         <f>E2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"="&amp;D2&amp;F2</f>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=1,DegreePlanID=10,TermId=1,RequirementId=560},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=1,DegreePlanID=10,TermID=1,RequirementID=560},</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2209,14 +2201,14 @@
         <v>542</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G66" si="0">E3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;","&amp;$D$1&amp;"="&amp;D3&amp;F3</f>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=2,DegreePlanID=10,TermId=1,RequirementId=542},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=2,DegreePlanID=10,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2233,14 +2225,14 @@
         <v>563</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=3,DegreePlanID=10,TermId=1,RequirementId=563},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=3,DegreePlanID=10,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2257,14 +2249,14 @@
         <v>555</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=4,DegreePlanID=10,TermId=2,RequirementId=555},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=4,DegreePlanID=10,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2281,14 +2273,14 @@
         <v>618</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=5,DegreePlanID=10,TermId=2,RequirementId=618},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=5,DegreePlanID=10,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2305,14 +2297,14 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=6,DegreePlanID=10,TermId=3,RequirementId=1},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=6,DegreePlanID=10,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2329,14 +2321,14 @@
         <v>664</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=7,DegreePlanID=10,TermId=3,RequirementId=664},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=7,DegreePlanID=10,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2353,14 +2345,14 @@
         <v>691</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=8,DegreePlanID=10,TermId=3,RequirementId=691},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=8,DegreePlanID=10,TermID=3,RequirementID=691},</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2377,14 +2369,14 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=9,DegreePlanID=10,TermId=4,RequirementId=10},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=9,DegreePlanID=10,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2401,14 +2393,14 @@
         <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=10,DegreePlanID=10,TermId=4,RequirementId=20},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=10,DegreePlanID=10,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2425,14 +2417,14 @@
         <v>692</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=11,DegreePlanID=10,TermId=5,RequirementId=692},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=11,DegreePlanID=10,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2449,14 +2441,14 @@
         <v>560</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F13" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=12,DegreePlanID=11,TermId=1,RequirementId=560},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=12,DegreePlanID=11,TermID=1,RequirementID=560},</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2473,14 +2465,14 @@
         <v>542</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=13,DegreePlanID=11,TermId=1,RequirementId=542},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=13,DegreePlanID=11,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2497,14 +2489,14 @@
         <v>563</v>
       </c>
       <c r="E15" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=14,DegreePlanID=11,TermId=1,RequirementId=563},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=14,DegreePlanID=11,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2521,14 +2513,14 @@
         <v>555</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F16" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=15,DegreePlanID=11,TermId=2,RequirementId=555},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=15,DegreePlanID=11,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2545,14 +2537,14 @@
         <v>618</v>
       </c>
       <c r="E17" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F17" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=16,DegreePlanID=11,TermId=2,RequirementId=618},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=16,DegreePlanID=11,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2569,14 +2561,14 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=17,DegreePlanID=11,TermId=2,RequirementId=1},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=17,DegreePlanID=11,TermID=2,RequirementID=1},</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2593,14 +2585,14 @@
         <v>664</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=18,DegreePlanID=11,TermId=4,RequirementId=664},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=18,DegreePlanID=11,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2617,14 +2609,14 @@
         <v>691</v>
       </c>
       <c r="E20" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=19,DegreePlanID=11,TermId=4,RequirementId=691},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=19,DegreePlanID=11,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2641,14 +2633,14 @@
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=20,DegreePlanID=11,TermId=4,RequirementId=10},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=20,DegreePlanID=11,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2665,14 +2657,14 @@
         <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F22" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=21,DegreePlanID=11,TermId=5,RequirementId=20},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=21,DegreePlanID=11,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2689,14 +2681,14 @@
         <v>692</v>
       </c>
       <c r="E23" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F23" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=22,DegreePlanID=11,TermId=5,RequirementId=692},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=22,DegreePlanID=11,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2713,14 +2705,14 @@
         <v>560</v>
       </c>
       <c r="E24" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F24" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=23,DegreePlanID=12,TermId=1,RequirementId=560},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=23,DegreePlanID=12,TermID=1,RequirementID=560},</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2737,14 +2729,14 @@
         <v>542</v>
       </c>
       <c r="E25" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F25" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=24,DegreePlanID=12,TermId=1,RequirementId=542},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=24,DegreePlanID=12,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2761,14 +2753,14 @@
         <v>563</v>
       </c>
       <c r="E26" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F26" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=25,DegreePlanID=12,TermId=1,RequirementId=563},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=25,DegreePlanID=12,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2785,14 +2777,14 @@
         <v>555</v>
       </c>
       <c r="E27" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F27" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=26,DegreePlanID=12,TermId=2,RequirementId=555},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=26,DegreePlanID=12,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2809,14 +2801,14 @@
         <v>618</v>
       </c>
       <c r="E28" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F28" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=27,DegreePlanID=12,TermId=2,RequirementId=618},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=27,DegreePlanID=12,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2833,14 +2825,14 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F29" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=28,DegreePlanID=12,TermId=3,RequirementId=1},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=28,DegreePlanID=12,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2857,14 +2849,14 @@
         <v>664</v>
       </c>
       <c r="E30" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F30" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=29,DegreePlanID=12,TermId=3,RequirementId=664},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=29,DegreePlanID=12,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2881,14 +2873,14 @@
         <v>691</v>
       </c>
       <c r="E31" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F31" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=30,DegreePlanID=12,TermId=3,RequirementId=691},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=30,DegreePlanID=12,TermID=3,RequirementID=691},</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2905,14 +2897,14 @@
         <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F32" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=31,DegreePlanID=12,TermId=4,RequirementId=10},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=31,DegreePlanID=12,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2929,14 +2921,14 @@
         <v>20</v>
       </c>
       <c r="E33" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F33" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=32,DegreePlanID=12,TermId=4,RequirementId=20},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=32,DegreePlanID=12,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2953,14 +2945,14 @@
         <v>692</v>
       </c>
       <c r="E34" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F34" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=33,DegreePlanID=12,TermId=5,RequirementId=692},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=33,DegreePlanID=12,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2977,14 +2969,14 @@
         <v>560</v>
       </c>
       <c r="E35" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F35" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=34,DegreePlanID=13,TermId=1,RequirementId=560},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=34,DegreePlanID=13,TermID=1,RequirementID=560},</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -3001,14 +2993,14 @@
         <v>542</v>
       </c>
       <c r="E36" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F36" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=35,DegreePlanID=13,TermId=1,RequirementId=542},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=35,DegreePlanID=13,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -3025,14 +3017,14 @@
         <v>563</v>
       </c>
       <c r="E37" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F37" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=36,DegreePlanID=13,TermId=1,RequirementId=563},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=36,DegreePlanID=13,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3049,14 +3041,14 @@
         <v>555</v>
       </c>
       <c r="E38" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F38" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=37,DegreePlanID=13,TermId=3,RequirementId=555},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=37,DegreePlanID=13,TermID=3,RequirementID=555},</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3073,14 +3065,14 @@
         <v>618</v>
       </c>
       <c r="E39" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F39" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=38,DegreePlanID=13,TermId=3,RequirementId=618},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=38,DegreePlanID=13,TermID=3,RequirementID=618},</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3097,14 +3089,14 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F40" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=39,DegreePlanID=13,TermId=3,RequirementId=1},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=39,DegreePlanID=13,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -3121,14 +3113,14 @@
         <v>664</v>
       </c>
       <c r="E41" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F41" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=40,DegreePlanID=13,TermId=4,RequirementId=664},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=40,DegreePlanID=13,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3145,14 +3137,14 @@
         <v>691</v>
       </c>
       <c r="E42" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F42" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=41,DegreePlanID=13,TermId=4,RequirementId=691},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=41,DegreePlanID=13,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -3169,14 +3161,14 @@
         <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F43" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=42,DegreePlanID=13,TermId=4,RequirementId=10},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=42,DegreePlanID=13,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3193,14 +3185,14 @@
         <v>20</v>
       </c>
       <c r="E44" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F44" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=43,DegreePlanID=13,TermId=5,RequirementId=20},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=43,DegreePlanID=13,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -3217,14 +3209,14 @@
         <v>692</v>
       </c>
       <c r="E45" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F45" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=44,DegreePlanID=13,TermId=5,RequirementId=692},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=44,DegreePlanID=13,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3241,14 +3233,14 @@
         <v>560</v>
       </c>
       <c r="E46" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F46" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=45,DegreePlanID=14,TermId=1,RequirementId=560},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=45,DegreePlanID=14,TermID=1,RequirementID=560},</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -3265,14 +3257,14 @@
         <v>542</v>
       </c>
       <c r="E47" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F47" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=46,DegreePlanID=14,TermId=1,RequirementId=542},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=46,DegreePlanID=14,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -3289,14 +3281,14 @@
         <v>563</v>
       </c>
       <c r="E48" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F48" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=47,DegreePlanID=14,TermId=1,RequirementId=563},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=47,DegreePlanID=14,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3313,14 +3305,14 @@
         <v>555</v>
       </c>
       <c r="E49" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F49" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=48,DegreePlanID=14,TermId=2,RequirementId=555},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=48,DegreePlanID=14,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -3337,14 +3329,14 @@
         <v>618</v>
       </c>
       <c r="E50" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F50" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=49,DegreePlanID=14,TermId=2,RequirementId=618},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=49,DegreePlanID=14,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -3361,14 +3353,14 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F51" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=50,DegreePlanID=14,TermId=3,RequirementId=1},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=50,DegreePlanID=14,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3385,14 +3377,14 @@
         <v>664</v>
       </c>
       <c r="E52" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F52" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=51,DegreePlanID=14,TermId=3,RequirementId=664},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=51,DegreePlanID=14,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3409,14 +3401,14 @@
         <v>691</v>
       </c>
       <c r="E53" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F53" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=52,DegreePlanID=14,TermId=3,RequirementId=691},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=52,DegreePlanID=14,TermID=3,RequirementID=691},</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -3433,14 +3425,14 @@
         <v>10</v>
       </c>
       <c r="E54" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F54" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=53,DegreePlanID=14,TermId=4,RequirementId=10},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=53,DegreePlanID=14,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -3457,14 +3449,14 @@
         <v>20</v>
       </c>
       <c r="E55" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F55" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=54,DegreePlanID=14,TermId=4,RequirementId=20},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=54,DegreePlanID=14,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -3481,14 +3473,14 @@
         <v>692</v>
       </c>
       <c r="E56" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F56" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=55,DegreePlanID=14,TermId=5,RequirementId=692},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=55,DegreePlanID=14,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3505,14 +3497,14 @@
         <v>560</v>
       </c>
       <c r="E57" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F57" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=56,DegreePlanID=15,TermId=1,RequirementId=560},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=56,DegreePlanID=15,TermID=1,RequirementID=560},</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -3529,14 +3521,14 @@
         <v>542</v>
       </c>
       <c r="E58" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F58" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=57,DegreePlanID=15,TermId=1,RequirementId=542},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=57,DegreePlanID=15,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3553,14 +3545,14 @@
         <v>563</v>
       </c>
       <c r="E59" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F59" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G59" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=58,DegreePlanID=15,TermId=1,RequirementId=563},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=58,DegreePlanID=15,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -3577,14 +3569,14 @@
         <v>555</v>
       </c>
       <c r="E60" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F60" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=59,DegreePlanID=15,TermId=2,RequirementId=555},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=59,DegreePlanID=15,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -3601,14 +3593,14 @@
         <v>618</v>
       </c>
       <c r="E61" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F61" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=60,DegreePlanID=15,TermId=2,RequirementId=618},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=60,DegreePlanID=15,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3625,14 +3617,14 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F62" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=61,DegreePlanID=15,TermId=2,RequirementId=1},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=61,DegreePlanID=15,TermID=2,RequirementID=1},</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3649,14 +3641,14 @@
         <v>664</v>
       </c>
       <c r="E63" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F63" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=62,DegreePlanID=15,TermId=4,RequirementId=664},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=62,DegreePlanID=15,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3673,14 +3665,14 @@
         <v>691</v>
       </c>
       <c r="E64" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F64" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=63,DegreePlanID=15,TermId=4,RequirementId=691},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=63,DegreePlanID=15,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3697,14 +3689,14 @@
         <v>10</v>
       </c>
       <c r="E65" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F65" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=64,DegreePlanID=15,TermId=4,RequirementId=10},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=64,DegreePlanID=15,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3721,14 +3713,14 @@
         <v>20</v>
       </c>
       <c r="E66" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F66" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=65,DegreePlanID=15,TermId=5,RequirementId=20},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=65,DegreePlanID=15,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3745,14 +3737,14 @@
         <v>692</v>
       </c>
       <c r="E67" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F67" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G67" t="str">
         <f t="shared" ref="G67:G89" si="1">E67&amp;$A$1&amp;"="&amp;A67&amp;","&amp;$B$1&amp;"="&amp;B67&amp;","&amp;$C$1&amp;"="&amp;C67&amp;","&amp;$D$1&amp;"="&amp;D67&amp;F67</f>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=66,DegreePlanID=15,TermId=5,RequirementId=692},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=66,DegreePlanID=15,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3769,14 +3761,14 @@
         <v>560</v>
       </c>
       <c r="E68" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F68" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=67,DegreePlanID=16,TermId=1,RequirementId=560},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=67,DegreePlanID=16,TermID=1,RequirementID=560},</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3793,14 +3785,14 @@
         <v>542</v>
       </c>
       <c r="E69" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F69" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=68,DegreePlanID=16,TermId=1,RequirementId=542},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=68,DegreePlanID=16,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3817,14 +3809,14 @@
         <v>563</v>
       </c>
       <c r="E70" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F70" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=69,DegreePlanID=16,TermId=1,RequirementId=563},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=69,DegreePlanID=16,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -3841,14 +3833,14 @@
         <v>555</v>
       </c>
       <c r="E71" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F71" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=70,DegreePlanID=16,TermId=2,RequirementId=555},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=70,DegreePlanID=16,TermID=2,RequirementID=555},</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3865,14 +3857,14 @@
         <v>618</v>
       </c>
       <c r="E72" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F72" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=71,DegreePlanID=16,TermId=2,RequirementId=618},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=71,DegreePlanID=16,TermID=2,RequirementID=618},</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3889,14 +3881,14 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F73" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=72,DegreePlanID=16,TermId=3,RequirementId=1},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=72,DegreePlanID=16,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3913,14 +3905,14 @@
         <v>664</v>
       </c>
       <c r="E74" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F74" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=73,DegreePlanID=16,TermId=3,RequirementId=664},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=73,DegreePlanID=16,TermID=3,RequirementID=664},</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3937,14 +3929,14 @@
         <v>691</v>
       </c>
       <c r="E75" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F75" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=74,DegreePlanID=16,TermId=4,RequirementId=691},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=74,DegreePlanID=16,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -3961,14 +3953,14 @@
         <v>10</v>
       </c>
       <c r="E76" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F76" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=75,DegreePlanID=16,TermId=4,RequirementId=10},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=75,DegreePlanID=16,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -3985,14 +3977,14 @@
         <v>20</v>
       </c>
       <c r="E77" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F77" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=76,DegreePlanID=16,TermId=4,RequirementId=20},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=76,DegreePlanID=16,TermID=4,RequirementID=20},</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -4009,14 +4001,14 @@
         <v>692</v>
       </c>
       <c r="E78" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F78" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G78" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=77,DegreePlanID=16,TermId=5,RequirementId=692},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=77,DegreePlanID=16,TermID=5,RequirementID=692},</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -4033,14 +4025,14 @@
         <v>560</v>
       </c>
       <c r="E79" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F79" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G79" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=78,DegreePlanID=17,TermId=1,RequirementId=560},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=78,DegreePlanID=17,TermID=1,RequirementID=560},</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -4057,14 +4049,14 @@
         <v>542</v>
       </c>
       <c r="E80" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F80" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G80" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=79,DegreePlanID=17,TermId=1,RequirementId=542},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=79,DegreePlanID=17,TermID=1,RequirementID=542},</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -4081,14 +4073,14 @@
         <v>563</v>
       </c>
       <c r="E81" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F81" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G81" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=80,DegreePlanID=17,TermId=1,RequirementId=563},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=80,DegreePlanID=17,TermID=1,RequirementID=563},</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -4105,14 +4097,14 @@
         <v>555</v>
       </c>
       <c r="E82" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F82" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G82" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=81,DegreePlanID=17,TermId=3,RequirementId=555},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=81,DegreePlanID=17,TermID=3,RequirementID=555},</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -4129,14 +4121,14 @@
         <v>618</v>
       </c>
       <c r="E83" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F83" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G83" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=82,DegreePlanID=17,TermId=3,RequirementId=618},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=82,DegreePlanID=17,TermID=3,RequirementID=618},</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -4153,14 +4145,14 @@
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F84" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G84" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=83,DegreePlanID=17,TermId=3,RequirementId=1},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=83,DegreePlanID=17,TermID=3,RequirementID=1},</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4177,14 +4169,14 @@
         <v>664</v>
       </c>
       <c r="E85" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F85" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G85" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=84,DegreePlanID=17,TermId=4,RequirementId=664},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=84,DegreePlanID=17,TermID=4,RequirementID=664},</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4201,14 +4193,14 @@
         <v>691</v>
       </c>
       <c r="E86" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F86" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G86" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=85,DegreePlanID=17,TermId=4,RequirementId=691},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=85,DegreePlanID=17,TermID=4,RequirementID=691},</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -4225,14 +4217,14 @@
         <v>10</v>
       </c>
       <c r="E87" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F87" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G87" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=86,DegreePlanID=17,TermId=4,RequirementId=10},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=86,DegreePlanID=17,TermID=4,RequirementID=10},</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -4249,14 +4241,14 @@
         <v>20</v>
       </c>
       <c r="E88" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F88" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G88" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=87,DegreePlanID=17,TermId=5,RequirementId=20},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=87,DegreePlanID=17,TermID=5,RequirementID=20},</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -4273,14 +4265,14 @@
         <v>692</v>
       </c>
       <c r="E89" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F89" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G89" t="str">
         <f t="shared" si="1"/>
-        <v>new Model.DegreePlanTermRequirement{DegreePlanTermRequirementId=88,DegreePlanID=17,TermId=5,RequirementId=692},</v>
+        <v>new Models.DegreePlanTermRequirement{DegreePlanTermRequirementID=88,DegreePlanID=17,TermID=5,RequirementID=692},</v>
       </c>
     </row>
   </sheetData>
@@ -4298,36 +4290,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="E1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="F1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="H1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -4341,20 +4333,20 @@
         <v>531441</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H2" t="str">
-        <f>F2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"="&amp;D2&amp;","&amp;$E$1&amp;"="&amp;E2&amp;G2</f>
-        <v>new Model.DegreePlan{DegreePlanId=10,DegreeID=4,StudentId=531441,DegreePlanAbbrev=No summer off,DegreePlanName=As Fast as I Can},</v>
+        <f>F2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"="&amp;D2&amp;""&amp;$E$1&amp;"="""&amp;E2&amp;G2</f>
+        <v>new Models.DegreePlan{DegreePlanID=10,DegreeID=4,StudentID=531441,DegreePlanAbbrev=No summer offDegreePlanName="As Fast as I Can},</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4368,20 +4360,20 @@
         <v>531441</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H9" si="0">F3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;","&amp;$D$1&amp;"="&amp;D3&amp;","&amp;$E$1&amp;"="&amp;E3&amp;G3</f>
-        <v>new Model.DegreePlan{DegreePlanId=11,DegreeID=4,StudentId=531441,DegreePlanAbbrev=Summer Off,DegreePlanName=Slow and Easy},</v>
+        <v>new Models.DegreePlan{DegreePlanID=11,DegreeID=4,StudentID=531441,DegreePlanAbbrev=Summer Off,DegreePlanName=Slow and Easy},</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4395,20 +4387,20 @@
         <v>531524</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlan{DegreePlanId=12,DegreeID=4,StudentId=531524,DegreePlanAbbrev=No summer off,DegreePlanName=As Fast as I Can},</v>
+        <v>new Models.DegreePlan{DegreePlanID=12,DegreeID=4,StudentID=531524,DegreePlanAbbrev=No summer off,DegreePlanName=As Fast as I Can},</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4422,20 +4414,20 @@
         <v>531524</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlan{DegreePlanId=13,DegreeID=4,StudentId=531524,DegreePlanAbbrev=Summer Off,DegreePlanName=Slow and Easy},</v>
+        <v>new Models.DegreePlan{DegreePlanID=13,DegreeID=4,StudentID=531524,DegreePlanAbbrev=Summer Off,DegreePlanName=Slow and Easy},</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4449,20 +4441,20 @@
         <v>531506</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G6" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlan{DegreePlanId=14,DegreeID=4,StudentId=531506,DegreePlanAbbrev=No summer off,DegreePlanName=As Fast as I Can},</v>
+        <v>new Models.DegreePlan{DegreePlanID=14,DegreeID=4,StudentID=531506,DegreePlanAbbrev=No summer off,DegreePlanName=As Fast as I Can},</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4476,20 +4468,20 @@
         <v>531506</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlan{DegreePlanId=15,DegreeID=4,StudentId=531506,DegreePlanAbbrev=Summer Off,DegreePlanName=Slow and Easy},</v>
+        <v>new Models.DegreePlan{DegreePlanID=15,DegreeID=4,StudentID=531506,DegreePlanAbbrev=Summer Off,DegreePlanName=Slow and Easy},</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4503,20 +4495,20 @@
         <v>530469</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G8" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlan{DegreePlanId=16,DegreeID=4,StudentId=530469,DegreePlanAbbrev=No summer off,DegreePlanName=As Fast as I Can},</v>
+        <v>new Models.DegreePlan{DegreePlanID=16,DegreeID=4,StudentID=530469,DegreePlanAbbrev=No summer off,DegreePlanName=As Fast as I Can},</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4530,20 +4522,20 @@
         <v>530469</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G9" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.DegreePlan{DegreePlanId=17,DegreeID=4,StudentId=530469,DegreePlanAbbrev=Summer Off,DegreePlanName=Slow and Easy},</v>
+        <v>new Models.DegreePlan{DegreePlanID=17,DegreeID=4,StudentID=530469,DegreePlanAbbrev=Summer Off,DegreePlanName=Slow and Easy},</v>
       </c>
     </row>
   </sheetData>
@@ -4555,9 +4547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4566,28 +4556,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" t="s">
-        <v>51</v>
-      </c>
       <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1">
-        <v>919</v>
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>87</v>
       </c>
       <c r="F1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="H1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -4595,10 +4585,10 @@
         <v>531441</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D2">
         <v>531441</v>
@@ -4607,14 +4597,14 @@
         <v>919562404</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H2" t="str">
         <f>F2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"="&amp;D2&amp;","&amp;$E$1&amp;"="&amp;E2&amp;G2</f>
-        <v>new Model.Student{StudentId=531441,First=Vyshnavi srilaxmi ,Last=Thannir,Snumber=531441,919=919562404},</v>
+        <v>new Models.Student{StudentID=531441,First=Vyshnavi srilaxmi ,Last=Thannir,Snumber=531441,SID=919562404},</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4622,10 +4612,10 @@
         <v>531524</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D3">
         <v>531524</v>
@@ -4634,14 +4624,14 @@
         <v>919562444</v>
       </c>
       <c r="F3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H5" si="0">F3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;","&amp;$D$1&amp;"="&amp;D3&amp;","&amp;$E$1&amp;"="&amp;E3&amp;G3</f>
-        <v>new Model.Student{StudentId=531524,First=Sri Ram Teja,Last=Komerisetti,Snumber=531524,919=919562444},</v>
+        <v>new Models.Student{StudentID=531524,First=Sri Ram Teja,Last=Komerisetti,Snumber=531524,SID=919562444},</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4649,10 +4639,10 @@
         <v>530469</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D4">
         <v>530469</v>
@@ -4661,14 +4651,14 @@
         <v>919559547</v>
       </c>
       <c r="F4" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="G4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.Student{StudentId=530469,First=Chandra Mouli,Last=Kantipudi,Snumber=530469,919=919559547},</v>
+        <v>new Models.Student{StudentID=530469,First=Chandra Mouli,Last=Kantipudi,Snumber=530469,SID=919559547},</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4676,10 +4666,10 @@
         <v>531506</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D5">
         <v>531506</v>
@@ -4688,14 +4678,14 @@
         <v>919562179</v>
       </c>
       <c r="F5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="G5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>new Model.Student{StudentId=531506,First=Prashanth Kumar,Last=Thallada,Snumber=531506,919=919562179},</v>
+        <v>new Models.Student{StudentID=531506,First=Prashanth Kumar,Last=Thallada,Snumber=531506,SID=919562179},</v>
       </c>
     </row>
   </sheetData>
@@ -4713,31 +4703,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="5.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4751,17 +4742,17 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G2" t="str">
         <f>E2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"="&amp;D2&amp;F2</f>
-        <v>new StudentTerm{StudentTermId=1,StudentID=531441,Term=1,Term Label=Fall 2017},</v>
+        <v>new Models.StudentTerm{StudentTermID=1,StudentID=531441,TermID=1,TermLabel=Fall 2017},</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4775,17 +4766,17 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G21" si="0">E3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;","&amp;$D$1&amp;"="&amp;D3&amp;F3</f>
-        <v>new StudentTerm{StudentTermId=2,StudentID=531441,Term=2,Term Label=Spring 2018},</v>
+        <v>new Models.StudentTerm{StudentTermID=2,StudentID=531441,TermID=2,TermLabel=Spring 2018},</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4799,17 +4790,17 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=3,StudentID=531441,Term=3,Term Label=Summer 2018},</v>
+        <v>new Models.StudentTerm{StudentTermID=3,StudentID=531441,TermID=3,TermLabel=Summer 2018},</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4823,17 +4814,17 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=4,StudentID=531441,Term=4,Term Label=Fall 2018},</v>
+        <v>new Models.StudentTerm{StudentTermID=4,StudentID=531441,TermID=4,TermLabel=Fall 2018},</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -4847,17 +4838,17 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=5,StudentID=531441,Term=5,Term Label=Spring 2019},</v>
+        <v>new Models.StudentTerm{StudentTermID=5,StudentID=531441,TermID=5,TermLabel=Spring 2019},</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -4871,17 +4862,17 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=6,StudentID=531524,Term=1,Term Label=Spring 2018},</v>
+        <v>new Models.StudentTerm{StudentTermID=6,StudentID=531524,TermID=1,TermLabel=Spring 2018},</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -4895,17 +4886,17 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=7,StudentID=531524,Term=2,Term Label=Summer 2018},</v>
+        <v>new Models.StudentTerm{StudentTermID=7,StudentID=531524,TermID=2,TermLabel=Summer 2018},</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -4919,17 +4910,17 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=8,StudentID=531524,Term=3,Term Label=Fall 2018},</v>
+        <v>new Models.StudentTerm{StudentTermID=8,StudentID=531524,TermID=3,TermLabel=Fall 2018},</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4943,17 +4934,17 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=9,StudentID=531524,Term=4,Term Label=Spring 2019},</v>
+        <v>new Models.StudentTerm{StudentTermID=9,StudentID=531524,TermID=4,TermLabel=Spring 2019},</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -4967,17 +4958,17 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=10,StudentID=531524,Term=5,Term Label=Summer 2019},</v>
+        <v>new Models.StudentTerm{StudentTermID=10,StudentID=531524,TermID=5,TermLabel=Summer 2019},</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -4991,17 +4982,17 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F12" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=11,StudentID=530469,Term=1,Term Label=Fall 2018},</v>
+        <v>new Models.StudentTerm{StudentTermID=11,StudentID=530469,TermID=1,TermLabel=Fall 2018},</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -5015,17 +5006,17 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F13" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=12,StudentID=530469,Term=2,Term Label=Spring 2019},</v>
+        <v>new Models.StudentTerm{StudentTermID=12,StudentID=530469,TermID=2,TermLabel=Spring 2019},</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -5039,17 +5030,17 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=13,StudentID=530469,Term=3,Term Label=Summer 2019},</v>
+        <v>new Models.StudentTerm{StudentTermID=13,StudentID=530469,TermID=3,TermLabel=Summer 2019},</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -5063,17 +5054,17 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=14,StudentID=530469,Term=4,Term Label=Fall 2019},</v>
+        <v>new Models.StudentTerm{StudentTermID=14,StudentID=530469,TermID=4,TermLabel=Fall 2019},</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -5087,17 +5078,17 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F16" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=15,StudentID=530469,Term=5,Term Label=Spring 2020},</v>
+        <v>new Models.StudentTerm{StudentTermID=15,StudentID=530469,TermID=5,TermLabel=Spring 2020},</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -5111,17 +5102,17 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F17" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=16,StudentID=531506,Term=1,Term Label=Spring 2020},</v>
+        <v>new Models.StudentTerm{StudentTermID=16,StudentID=531506,TermID=1,TermLabel=Spring 2020},</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -5135,17 +5126,17 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E18" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=17,StudentID=531506,Term=2,Term Label=Summer 2020},</v>
+        <v>new Models.StudentTerm{StudentTermID=17,StudentID=531506,TermID=2,TermLabel=Summer 2020},</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -5159,17 +5150,17 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=18,StudentID=531506,Term=3,Term Label=Fall 2020},</v>
+        <v>new Models.StudentTerm{StudentTermID=18,StudentID=531506,TermID=3,TermLabel=Fall 2020},</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -5183,17 +5174,17 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E20" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=19,StudentID=531506,Term=4,Term Label=Spring 2021},</v>
+        <v>new Models.StudentTerm{StudentTermID=19,StudentID=531506,TermID=4,TermLabel=Spring 2021},</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -5207,17 +5198,17 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm{StudentTermId=20,StudentID=531506,Term=5,Term Label=Summer 2021},</v>
+        <v>new Models.StudentTerm{StudentTermID=20,StudentID=531506,TermID=5,TermLabel=Summer 2021},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>